<commit_message>
Updated for new stories for stall registration.
</commit_message>
<xml_diff>
--- a/Documents/APMC Task BreakUp.xlsx
+++ b/Documents/APMC Task BreakUp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Office\APMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Office\APMC\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F04E78-2B4F-4626-A64F-AF63B8898368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CF8BAF-CD84-4C66-A1FC-1796D33E8959}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Complexity &amp; Prority" sheetId="5" r:id="rId5"/>
+    <sheet name="Points" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="248">
   <si>
     <t>LANGUAGES--ENGLISH AND MARATHI</t>
   </si>
@@ -757,13 +758,37 @@
   </si>
   <si>
     <t>Estimation</t>
+  </si>
+  <si>
+    <t>Sign Up Page</t>
+  </si>
+  <si>
+    <t>Pradnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stall Registration for New Merchant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stall Registration for  Existing Merchant </t>
+  </si>
+  <si>
+    <t>Points to add to the excel sheet:</t>
+  </si>
+  <si>
+    <t>1. Reset password after 90 days.</t>
+  </si>
+  <si>
+    <t>2. Ask user to reset password after three unsuccessfull attempts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Andriod/ iOS phone versions that are compatible with APMC app. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +848,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -901,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -962,13 +995,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2548,12 +2588,12 @@
     </row>
     <row r="3" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -3185,10 +3225,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764A796D-AF83-44AA-B6FB-C14DAD962DF1}">
-  <dimension ref="B3:XFD23"/>
+  <dimension ref="B3:XFD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,8 +3262,8 @@
       <c r="H3" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
       <c r="XFD3" t="s">
         <v>238</v>
       </c>
@@ -3239,7 +3279,7 @@
         <v>201</v>
       </c>
       <c r="E4" s="15">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F4" s="15">
         <v>1</v>
@@ -3248,38 +3288,38 @@
         <v>200</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="2:10 16384:16384" x14ac:dyDescent="0.25">
       <c r="B5" s="15">
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E5" s="15">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="F5" s="15">
         <v>1</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="2:10 16384:16384" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
         <v>3</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>236</v>
@@ -3291,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H6" s="15"/>
     </row>
@@ -3300,19 +3340,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="E7" s="15">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="F7" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -3321,16 +3361,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E8" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>200</v>
@@ -3342,7 +3382,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>201</v>
@@ -3351,7 +3391,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>200</v>
@@ -3363,7 +3403,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>201</v>
@@ -3384,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>201</v>
@@ -3393,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>200</v>
@@ -3405,16 +3445,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E12" s="15">
+        <v>2</v>
+      </c>
+      <c r="F12" s="15">
         <v>4</v>
-      </c>
-      <c r="F12" s="15">
-        <v>5</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>200</v>
@@ -3426,16 +3466,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E13" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>200</v>
@@ -3447,7 +3487,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>201</v>
@@ -3468,16 +3508,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E15" s="15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="15">
         <v>3</v>
-      </c>
-      <c r="F15" s="15">
-        <v>2</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>200</v>
@@ -3489,16 +3529,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E16" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>200</v>
@@ -3510,16 +3550,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E17" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>200</v>
@@ -3531,19 +3571,19 @@
         <v>15</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E18" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18" s="15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H18" s="15"/>
     </row>
@@ -3552,16 +3592,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E19" s="15">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>199</v>
@@ -3573,7 +3613,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>102</v>
+        <v>228</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>201</v>
@@ -3594,63 +3634,142 @@
         <v>18</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E21" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" s="15">
         <v>2</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="H21" s="15"/>
+      <c r="G21" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>19</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E22" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F22" s="15">
         <v>2</v>
       </c>
-      <c r="F22" s="15">
-        <v>6</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="H22" s="15"/>
+      <c r="G22" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="15">
         <v>20</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>201</v>
       </c>
       <c r="E23" s="15">
+        <v>4</v>
+      </c>
+      <c r="F23" s="15">
         <v>2</v>
-      </c>
-      <c r="F23" s="15">
-        <v>6</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>199</v>
       </c>
       <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
+        <v>21</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="15">
+        <v>2</v>
+      </c>
+      <c r="F24" s="15">
+        <v>6</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
+        <v>22</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="15">
+        <v>2</v>
+      </c>
+      <c r="F25" s="15">
+        <v>6</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCFFB0B-09F2-4D0F-83AA-4C45E0DC1541}">
+  <dimension ref="D7:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>